<commit_message>
added people to gantn chart for week 1
</commit_message>
<xml_diff>
--- a/documents/EditorGant2016.xlsx
+++ b/documents/EditorGant2016.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Week</t>
   </si>
@@ -58,6 +61,15 @@
   </si>
   <si>
     <t>Serialization QA (code)</t>
+  </si>
+  <si>
+    <t>Zhipeng</t>
+  </si>
+  <si>
+    <t>George/Diana/Pranoy</t>
+  </si>
+  <si>
+    <t>George/Sunh/Wei</t>
   </si>
 </sst>
 </file>
@@ -120,8 +132,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -420,7 +460,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,20 +526,26 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>